<commit_message>
fix bug in inserting new companies and taf details
</commit_message>
<xml_diff>
--- a/RPA CA3 Group 2 Robot/Database1.xlsx
+++ b/RPA CA3 Group 2 Robot/Database1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rxlee\OneDrive\Desktop\Learning Resources\Y2 SEM 1\RPA\CA3\RPA CA3 git repo\RPA CA3 Group 2 Robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9798C7D5-D10F-424D-B018-50F6E35F977B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF7CCF3-18B0-470F-83DD-42475CE3DEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -999,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
update shortlist candidates :>
</commit_message>
<xml_diff>
--- a/RPA CA3 Group 2 Robot/Database1.xlsx
+++ b/RPA CA3 Group 2 Robot/Database1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rxlee\OneDrive\Desktop\Learning Resources\Y2 SEM 1\RPA\CA3\RPA CA3 git repo\RPA CA3 Group 2 Robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F9CCAE-06C3-4E0C-B310-B206AE538682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3451884C-CFA5-4A0B-837A-6B2666127B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
@@ -879,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1002,7 +1002,7 @@
   <dimension ref="A3:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1168,7 +1168,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1372,7 +1372,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1628,8 +1628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:J13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
email letter of employment and medical check up plus email the candidates that declined the offer
</commit_message>
<xml_diff>
--- a/RPA CA3 Group 2 Robot/Database1.xlsx
+++ b/RPA CA3 Group 2 Robot/Database1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rxlee\OneDrive\Desktop\Learning Resources\Y2 SEM 1\RPA\CA3\RPA CA3 git repo\RPA CA3 Group 2 Robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3451884C-CFA5-4A0B-837A-6B2666127B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750220DC-34BB-47DD-9B3C-C4B63DAA950F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
@@ -124,9 +124,6 @@
     <t>Country of Birth</t>
   </si>
   <si>
-    <t xml:space="preserve">Email </t>
-  </si>
-  <si>
     <t>Qualification</t>
   </si>
   <si>
@@ -437,6 +434,9 @@
   </si>
   <si>
     <t>Project Management, Financial Management</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
@@ -880,7 +880,7 @@
   <dimension ref="A3:G6"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -908,27 +908,27 @@
         <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" t="s">
         <v>126</v>
-      </c>
-      <c r="B4" t="s">
-        <v>127</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -937,21 +937,21 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -960,21 +960,21 @@
         <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -983,7 +983,7 @@
         <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1002,7 +1002,7 @@
   <dimension ref="A3:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1049,25 +1049,25 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C4" s="3">
         <v>44760</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H4" s="3">
         <v>44805</v>
@@ -1075,25 +1075,25 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5" s="3">
         <v>44805</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H5" s="3">
         <v>44819</v>
@@ -1101,60 +1101,60 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C6" s="3">
         <v>44835</v>
       </c>
       <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
         <v>52</v>
-      </c>
-      <c r="E6" t="s">
-        <v>53</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H6" s="3">
         <v>44880</v>
       </c>
       <c r="I6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C7" s="3">
         <v>44838</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H7" s="3">
         <v>44885</v>
       </c>
       <c r="I7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1168,7 +1168,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1186,7 +1186,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
@@ -1215,7 +1215,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>31</v>
+        <v>135</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>1</v>
@@ -1224,135 +1224,135 @@
         <v>0</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="3">
         <v>33761</v>
       </c>
       <c r="D4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="F4" t="s">
         <v>62</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="H4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I4">
         <v>98412378</v>
       </c>
       <c r="J4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C5" s="3">
         <v>33066</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E5" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
         <v>62</v>
       </c>
-      <c r="F5" t="s">
-        <v>63</v>
-      </c>
       <c r="G5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" t="s">
         <v>74</v>
-      </c>
-      <c r="H5" t="s">
-        <v>75</v>
       </c>
       <c r="I5">
         <v>96666666</v>
       </c>
       <c r="J5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" s="3">
         <v>24494</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="F6" t="s">
         <v>62</v>
       </c>
-      <c r="F6" t="s">
-        <v>63</v>
-      </c>
       <c r="G6" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" t="s">
         <v>81</v>
-      </c>
-      <c r="H6" t="s">
-        <v>82</v>
       </c>
       <c r="I6">
         <v>98888888</v>
       </c>
       <c r="J6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" s="3">
         <v>34853</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E7" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" t="s">
         <v>62</v>
       </c>
-      <c r="F7" t="s">
-        <v>63</v>
-      </c>
       <c r="G7" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" t="s">
         <v>91</v>
-      </c>
-      <c r="H7" t="s">
-        <v>92</v>
       </c>
       <c r="I7">
         <v>89999999</v>
       </c>
       <c r="J7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1390,7 +1390,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
@@ -1405,35 +1405,35 @@
         <v>26</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="D4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>36</v>
-      </c>
       <c r="F4" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H4" s="19"/>
       <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>68</v>
-      </c>
       <c r="C5" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" s="3">
         <v>41365</v>
@@ -1442,73 +1442,73 @@
         <v>43464</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="17"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" s="3">
         <v>43466</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="17"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>78</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>79</v>
       </c>
       <c r="D7" s="3">
         <v>40698</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="3">
         <v>34060</v>
@@ -1517,48 +1517,48 @@
         <v>37985</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>85</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>86</v>
       </c>
       <c r="D9" s="3">
         <v>37987</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D10" s="3">
         <v>43559</v>
@@ -1567,35 +1567,35 @@
         <v>44416</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D11" s="3">
         <v>44511</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1629,7 +1629,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1644,7 +1644,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="4" t="s">
@@ -1655,19 +1655,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>3</v>
@@ -1675,56 +1675,56 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" s="24">
         <v>44781</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6" s="24">
         <v>44782</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" s="24">
         <v>44814</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Whatsapp Arrange Interview
</commit_message>
<xml_diff>
--- a/RPA CA3 Group 2 Robot/Database1.xlsx
+++ b/RPA CA3 Group 2 Robot/Database1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rxlee\OneDrive\Desktop\Learning Resources\Y2 SEM 1\RPA\CA3\RPA CA3 git repo\RPA CA3 Group 2 Robot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaleb Nim\Documents\GitHub\RPA_grp2\RPA CA3 Group 2 Robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49674663-2ADB-4A47-A5B0-1E4418133491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8791D99F-E565-4D48-A80D-306390842CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="1485" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="220">
   <si>
     <t>HP</t>
   </si>
@@ -437,6 +437,259 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>C104</t>
+  </si>
+  <si>
+    <t>NEW COMPANY 1</t>
+  </si>
+  <si>
+    <t>50A Marine Ter #01-1511</t>
+  </si>
+  <si>
+    <t>6111 2222</t>
+  </si>
+  <si>
+    <t>Jennifer M Cohen</t>
+  </si>
+  <si>
+    <t>JenM@newComOne.com</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>C105</t>
+  </si>
+  <si>
+    <t>NEW COMPANY 2</t>
+  </si>
+  <si>
+    <t>203 Lorong Chuan</t>
+  </si>
+  <si>
+    <t>6333 4444</t>
+  </si>
+  <si>
+    <t>Timothy K Albertson</t>
+  </si>
+  <si>
+    <t>TimK@newComTwo.com</t>
+  </si>
+  <si>
+    <t>Executive Manager</t>
+  </si>
+  <si>
+    <t>TAF5</t>
+  </si>
+  <si>
+    <t>18/7/2022</t>
+  </si>
+  <si>
+    <t>HTML, CSS, JAVA, React, JQuery</t>
+  </si>
+  <si>
+    <t>TAF6</t>
+  </si>
+  <si>
+    <t>Actor</t>
+  </si>
+  <si>
+    <t>Work as a team, Reliable, Good Stage Presence</t>
+  </si>
+  <si>
+    <t>Height above 160cm</t>
+  </si>
+  <si>
+    <t>TAF7</t>
+  </si>
+  <si>
+    <t>19/5/2022</t>
+  </si>
+  <si>
+    <t>Producer</t>
+  </si>
+  <si>
+    <t>Produce scripts, Flexible work timings</t>
+  </si>
+  <si>
+    <t>13/8/2022</t>
+  </si>
+  <si>
+    <t>TAF8</t>
+  </si>
+  <si>
+    <t>Logistician</t>
+  </si>
+  <si>
+    <t>Problem Solving, Critical thinking, Communication</t>
+  </si>
+  <si>
+    <t>24/11/2022</t>
+  </si>
+  <si>
+    <t>ELEANOR FITZGERALD_x000D_</t>
+  </si>
+  <si>
+    <t>S6934567H</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>hello@reallygreatsite.com</t>
+  </si>
+  <si>
+    <t>Clementi Ave 6 #32-100_x000D_</t>
+  </si>
+  <si>
+    <t>87745560_x000D_</t>
+  </si>
+  <si>
+    <t>Bachelor of Computer Science - Software Engineering_x000D_</t>
+  </si>
+  <si>
+    <t>Kai Wen_x000D_</t>
+  </si>
+  <si>
+    <t>T0059829h</t>
+  </si>
+  <si>
+    <t>23/1/2000</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Kai_wen@gmail.com</t>
+  </si>
+  <si>
+    <t>Senkang Road 10 blk 12 #3-21_x000D_</t>
+  </si>
+  <si>
+    <t>92217949_x000D_</t>
+  </si>
+  <si>
+    <t>Diploma in statistics and marketing_x000D_</t>
+  </si>
+  <si>
+    <t>Penny Neo_x000D_</t>
+  </si>
+  <si>
+    <t>T0416829F</t>
+  </si>
+  <si>
+    <t>Penny_Neo@gmail.com</t>
+  </si>
+  <si>
+    <t>Woodlands Avenue blk 796 #5-307_x000D_</t>
+  </si>
+  <si>
+    <t>86855793_x000D_</t>
+  </si>
+  <si>
+    <t>Masters Of Science_x000D_</t>
+  </si>
+  <si>
+    <t>Ruo Xuan_x000D_</t>
+  </si>
+  <si>
+    <t>T0418324Z</t>
+  </si>
+  <si>
+    <t>24/7/2004</t>
+  </si>
+  <si>
+    <t>RuoXuan@gmail.com</t>
+  </si>
+  <si>
+    <t>Admiralty drive 20 blk 665 #5-307_x000D_</t>
+  </si>
+  <si>
+    <t>83992669_x000D_</t>
+  </si>
+  <si>
+    <t>Degree in Full-stack development_x000D_</t>
+  </si>
+  <si>
+    <t>Wardiere Inc._x000D_</t>
+  </si>
+  <si>
+    <t>Web Developer_x000D_</t>
+  </si>
+  <si>
+    <t>23/8/2021</t>
+  </si>
+  <si>
+    <t>JS,MongoDB,React,Next.js,Rust_x000D_,</t>
+  </si>
+  <si>
+    <t>Ensure user satisfaction and retention by providing responsive tech support._x000D_</t>
+  </si>
+  <si>
+    <t>Catalyst Inc. Singapore_x000D_</t>
+  </si>
+  <si>
+    <t>Data Analyst_x000D_</t>
+  </si>
+  <si>
+    <t>15/7/2021</t>
+  </si>
+  <si>
+    <t>Seaborn,Plotly,T ableau,R_x000D_</t>
+  </si>
+  <si>
+    <t>Plot revenue insights and deliever to plan future_x000D_</t>
+  </si>
+  <si>
+    <t>ABC Bank Singapore_x000D_</t>
+  </si>
+  <si>
+    <t>Advanced Analytics Manager_x000D_</t>
+  </si>
+  <si>
+    <t>T ableau,Python,Spark,R,SAS,SQL,MATLAB_x000D_</t>
+  </si>
+  <si>
+    <t>Drive consumeranalytics capabilities of consumer_x000D_</t>
+  </si>
+  <si>
+    <t>Project SP Inc._x000D_</t>
+  </si>
+  <si>
+    <t>Front-End-Web-Dev_x000D_</t>
+  </si>
+  <si>
+    <t>25/3/2017</t>
+  </si>
+  <si>
+    <t>React,React Native,HTML,Javascript,Node.js_x000D_</t>
+  </si>
+  <si>
+    <t>Make Company Website for marketing analaysis_x000D_</t>
+  </si>
+  <si>
+    <t>Arranging Interview</t>
+  </si>
+  <si>
+    <t>T0418191z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84953150
+</t>
+  </si>
+  <si>
+    <t>T0421062f</t>
+  </si>
+  <si>
+    <t>30/7/2022</t>
+  </si>
+  <si>
+    <t>1pm</t>
   </si>
 </sst>
 </file>
@@ -444,10 +697,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -548,7 +801,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -560,7 +813,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -571,8 +824,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -581,7 +834,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -875,24 +1128,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:G6"/>
+  <dimension ref="A3:G8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" customWidth="1"/>
-    <col min="2" max="2" width="32.36328125" customWidth="1"/>
-    <col min="3" max="3" width="39.453125" customWidth="1"/>
-    <col min="4" max="4" width="19.90625" customWidth="1"/>
-    <col min="5" max="5" width="26.7265625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="17.6328125" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -915,7 +1168,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -938,7 +1191,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -961,7 +1214,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -982,6 +1235,52 @@
       </c>
       <c r="G6" t="s">
         <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" t="s">
+        <v>148</v>
+      </c>
+      <c r="F8" t="s">
+        <v>149</v>
+      </c>
+      <c r="G8" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -997,26 +1296,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:I7"/>
+  <dimension ref="A3:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.7265625" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.6328125" customWidth="1"/>
-    <col min="5" max="5" width="37.08984375" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="37.140625" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" customWidth="1"/>
-    <col min="8" max="8" width="13.36328125" customWidth="1"/>
-    <col min="9" max="9" width="58.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="58.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>18</v>
       </c>
@@ -1045,7 +1344,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>41</v>
       </c>
@@ -1071,7 +1370,7 @@
         <v>44805</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>44</v>
       </c>
@@ -1097,7 +1396,7 @@
         <v>44819</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>50</v>
       </c>
@@ -1126,7 +1425,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>54</v>
       </c>
@@ -1153,6 +1452,113 @@
       </c>
       <c r="I7" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="3">
+        <v>44905</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="3">
+        <v>44568</v>
+      </c>
+      <c r="D9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E9" t="s">
+        <v>156</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="3">
+        <v>44569</v>
+      </c>
+      <c r="I9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" t="s">
+        <v>159</v>
+      </c>
+      <c r="D10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="3">
+        <v>44875</v>
+      </c>
+      <c r="D11" t="s">
+        <v>164</v>
+      </c>
+      <c r="E11" t="s">
+        <v>165</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1163,26 +1569,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8:I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" customWidth="1"/>
-    <col min="3" max="4" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="13.90625" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="19.08984375" customWidth="1"/>
-    <col min="8" max="8" width="30.36328125" customWidth="1"/>
-    <col min="9" max="9" width="14.6328125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
     <col min="10" max="10" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>107</v>
       </c>
@@ -1190,10 +1596,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1225,7 +1631,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -1257,7 +1663,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -1289,7 +1695,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>79</v>
       </c>
@@ -1321,7 +1727,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -1351,6 +1757,134 @@
       </c>
       <c r="J7" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="3">
+        <v>25326</v>
+      </c>
+      <c r="D8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" t="s">
+        <v>170</v>
+      </c>
+      <c r="H8" t="s">
+        <v>171</v>
+      </c>
+      <c r="I8" t="s">
+        <v>172</v>
+      </c>
+      <c r="J8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" t="s">
+        <v>177</v>
+      </c>
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" t="s">
+        <v>178</v>
+      </c>
+      <c r="H9" t="s">
+        <v>179</v>
+      </c>
+      <c r="I9" t="s">
+        <v>180</v>
+      </c>
+      <c r="J9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C10" s="3">
+        <v>38175</v>
+      </c>
+      <c r="D10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" t="s">
+        <v>184</v>
+      </c>
+      <c r="H10" t="s">
+        <v>185</v>
+      </c>
+      <c r="I10" t="s">
+        <v>186</v>
+      </c>
+      <c r="J10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D11" t="s">
+        <v>169</v>
+      </c>
+      <c r="E11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" t="s">
+        <v>191</v>
+      </c>
+      <c r="H11" t="s">
+        <v>192</v>
+      </c>
+      <c r="I11" t="s">
+        <v>193</v>
+      </c>
+      <c r="J11" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -1367,26 +1901,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:K18"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" customWidth="1"/>
-    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
     <col min="6" max="6" width="39" customWidth="1"/>
-    <col min="7" max="7" width="104.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.90625" customWidth="1"/>
-    <col min="9" max="9" width="44.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="104.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="44.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>105</v>
       </c>
@@ -1394,11 +1928,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H3" s="18"/>
       <c r="I3" s="17"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>26</v>
       </c>
@@ -1423,7 +1957,7 @@
       <c r="H4" s="19"/>
       <c r="I4" s="17"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>66</v>
       </c>
@@ -1448,7 +1982,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="17"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>66</v>
       </c>
@@ -1473,7 +2007,7 @@
       <c r="H6" s="19"/>
       <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>103</v>
       </c>
@@ -1498,7 +2032,7 @@
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>86</v>
       </c>
@@ -1523,7 +2057,7 @@
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>86</v>
       </c>
@@ -1548,7 +2082,7 @@
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>88</v>
       </c>
@@ -1573,7 +2107,7 @@
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>88</v>
       </c>
@@ -1594,6 +2128,98 @@
       </c>
       <c r="G11" s="11" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" t="s">
+        <v>195</v>
+      </c>
+      <c r="C12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" s="3">
+        <v>43927</v>
+      </c>
+      <c r="E12" t="s">
+        <v>197</v>
+      </c>
+      <c r="F12" t="s">
+        <v>198</v>
+      </c>
+      <c r="G12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D13" s="3">
+        <v>43288</v>
+      </c>
+      <c r="E13" t="s">
+        <v>202</v>
+      </c>
+      <c r="F13" t="s">
+        <v>203</v>
+      </c>
+      <c r="G13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B14" t="s">
+        <v>205</v>
+      </c>
+      <c r="C14" t="s">
+        <v>206</v>
+      </c>
+      <c r="D14" s="3">
+        <v>43288</v>
+      </c>
+      <c r="E14" t="s">
+        <v>202</v>
+      </c>
+      <c r="F14" t="s">
+        <v>207</v>
+      </c>
+      <c r="G14" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>189</v>
+      </c>
+      <c r="B15" t="s">
+        <v>209</v>
+      </c>
+      <c r="C15" t="s">
+        <v>210</v>
+      </c>
+      <c r="D15" t="s">
+        <v>211</v>
+      </c>
+      <c r="E15" s="3">
+        <v>43558</v>
+      </c>
+      <c r="F15" t="s">
+        <v>212</v>
+      </c>
+      <c r="G15" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -1604,23 +2230,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="19.90625" customWidth="1"/>
-    <col min="3" max="3" width="14.36328125" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>106</v>
       </c>
@@ -1631,7 +2258,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
@@ -1650,8 +2277,11 @@
       <c r="F4" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
@@ -1668,8 +2298,11 @@
       <c r="F5" s="14" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5">
+        <v>86553140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
@@ -1686,8 +2319,11 @@
       <c r="F6" s="14" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6">
+        <v>91874123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>44</v>
       </c>
@@ -1703,6 +2339,43 @@
       <c r="E7" s="14"/>
       <c r="F7" s="14" t="s">
         <v>131</v>
+      </c>
+      <c r="G7">
+        <v>88564432</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" s="3">
+        <v>44814</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C9" t="s">
+        <v>218</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="G9">
+        <v>83992669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more Resume to match TAF
</commit_message>
<xml_diff>
--- a/RPA CA3 Group 2 Robot/Database1.xlsx
+++ b/RPA CA3 Group 2 Robot/Database1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaleb Nim\Documents\GitHub\RPA_grp2\RPA CA3 Group 2 Robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8791D99F-E565-4D48-A80D-306390842CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7ECD6C7-12F8-4054-BE1B-89DA657752C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="1485" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="1485" windowWidth="23175" windowHeight="11400" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="166">
   <si>
     <t>HP</t>
   </si>
@@ -439,9 +439,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
     <t>C104</t>
   </si>
   <si>
@@ -530,166 +527,6 @@
   </si>
   <si>
     <t>24/11/2022</t>
-  </si>
-  <si>
-    <t>ELEANOR FITZGERALD_x000D_</t>
-  </si>
-  <si>
-    <t>S6934567H</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>hello@reallygreatsite.com</t>
-  </si>
-  <si>
-    <t>Clementi Ave 6 #32-100_x000D_</t>
-  </si>
-  <si>
-    <t>87745560_x000D_</t>
-  </si>
-  <si>
-    <t>Bachelor of Computer Science - Software Engineering_x000D_</t>
-  </si>
-  <si>
-    <t>Kai Wen_x000D_</t>
-  </si>
-  <si>
-    <t>T0059829h</t>
-  </si>
-  <si>
-    <t>23/1/2000</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Kai_wen@gmail.com</t>
-  </si>
-  <si>
-    <t>Senkang Road 10 blk 12 #3-21_x000D_</t>
-  </si>
-  <si>
-    <t>92217949_x000D_</t>
-  </si>
-  <si>
-    <t>Diploma in statistics and marketing_x000D_</t>
-  </si>
-  <si>
-    <t>Penny Neo_x000D_</t>
-  </si>
-  <si>
-    <t>T0416829F</t>
-  </si>
-  <si>
-    <t>Penny_Neo@gmail.com</t>
-  </si>
-  <si>
-    <t>Woodlands Avenue blk 796 #5-307_x000D_</t>
-  </si>
-  <si>
-    <t>86855793_x000D_</t>
-  </si>
-  <si>
-    <t>Masters Of Science_x000D_</t>
-  </si>
-  <si>
-    <t>Ruo Xuan_x000D_</t>
-  </si>
-  <si>
-    <t>T0418324Z</t>
-  </si>
-  <si>
-    <t>24/7/2004</t>
-  </si>
-  <si>
-    <t>RuoXuan@gmail.com</t>
-  </si>
-  <si>
-    <t>Admiralty drive 20 blk 665 #5-307_x000D_</t>
-  </si>
-  <si>
-    <t>83992669_x000D_</t>
-  </si>
-  <si>
-    <t>Degree in Full-stack development_x000D_</t>
-  </si>
-  <si>
-    <t>Wardiere Inc._x000D_</t>
-  </si>
-  <si>
-    <t>Web Developer_x000D_</t>
-  </si>
-  <si>
-    <t>23/8/2021</t>
-  </si>
-  <si>
-    <t>JS,MongoDB,React,Next.js,Rust_x000D_,</t>
-  </si>
-  <si>
-    <t>Ensure user satisfaction and retention by providing responsive tech support._x000D_</t>
-  </si>
-  <si>
-    <t>Catalyst Inc. Singapore_x000D_</t>
-  </si>
-  <si>
-    <t>Data Analyst_x000D_</t>
-  </si>
-  <si>
-    <t>15/7/2021</t>
-  </si>
-  <si>
-    <t>Seaborn,Plotly,T ableau,R_x000D_</t>
-  </si>
-  <si>
-    <t>Plot revenue insights and deliever to plan future_x000D_</t>
-  </si>
-  <si>
-    <t>ABC Bank Singapore_x000D_</t>
-  </si>
-  <si>
-    <t>Advanced Analytics Manager_x000D_</t>
-  </si>
-  <si>
-    <t>T ableau,Python,Spark,R,SAS,SQL,MATLAB_x000D_</t>
-  </si>
-  <si>
-    <t>Drive consumeranalytics capabilities of consumer_x000D_</t>
-  </si>
-  <si>
-    <t>Project SP Inc._x000D_</t>
-  </si>
-  <si>
-    <t>Front-End-Web-Dev_x000D_</t>
-  </si>
-  <si>
-    <t>25/3/2017</t>
-  </si>
-  <si>
-    <t>React,React Native,HTML,Javascript,Node.js_x000D_</t>
-  </si>
-  <si>
-    <t>Make Company Website for marketing analaysis_x000D_</t>
-  </si>
-  <si>
-    <t>Arranging Interview</t>
-  </si>
-  <si>
-    <t>T0418191z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84953150
-</t>
-  </si>
-  <si>
-    <t>T0421062f</t>
-  </si>
-  <si>
-    <t>30/7/2022</t>
-  </si>
-  <si>
-    <t>1pm</t>
   </si>
 </sst>
 </file>
@@ -1130,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:G8"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,48 +1076,48 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" t="s">
         <v>137</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>138</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>139</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>140</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>141</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>142</v>
-      </c>
-      <c r="G7" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" t="s">
         <v>144</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>145</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>146</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>147</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>148</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>149</v>
-      </c>
-      <c r="G8" t="s">
-        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1298,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,19 +1293,19 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
         <v>125</v>
       </c>
       <c r="C8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D8" t="s">
         <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -1482,19 +1319,19 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C9" s="3">
         <v>44568</v>
       </c>
       <c r="D9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" t="s">
         <v>155</v>
-      </c>
-      <c r="E9" t="s">
-        <v>156</v>
       </c>
       <c r="F9">
         <v>5</v>
@@ -1506,24 +1343,24 @@
         <v>44569</v>
       </c>
       <c r="I9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" t="s">
         <v>158</v>
       </c>
-      <c r="B10" t="s">
-        <v>137</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>159</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>160</v>
-      </c>
-      <c r="E10" t="s">
-        <v>161</v>
       </c>
       <c r="F10">
         <v>3</v>
@@ -1532,24 +1369,24 @@
         <v>47</v>
       </c>
       <c r="H10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C11" s="3">
         <v>44875</v>
       </c>
       <c r="D11" t="s">
+        <v>163</v>
+      </c>
+      <c r="E11" t="s">
         <v>164</v>
-      </c>
-      <c r="E11" t="s">
-        <v>165</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1558,7 +1395,7 @@
         <v>48</v>
       </c>
       <c r="H11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1569,17 +1406,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:I11"/>
+      <selection activeCell="A8" sqref="A8:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="4" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="19.140625" customWidth="1"/>
@@ -1592,9 +1430,7 @@
       <c r="A1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1757,134 +1593,6 @@
       </c>
       <c r="J7" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>167</v>
-      </c>
-      <c r="B8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C8" s="3">
-        <v>25326</v>
-      </c>
-      <c r="D8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" t="s">
-        <v>170</v>
-      </c>
-      <c r="H8" t="s">
-        <v>171</v>
-      </c>
-      <c r="I8" t="s">
-        <v>172</v>
-      </c>
-      <c r="J8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>174</v>
-      </c>
-      <c r="B9" t="s">
-        <v>175</v>
-      </c>
-      <c r="C9" t="s">
-        <v>176</v>
-      </c>
-      <c r="D9" t="s">
-        <v>177</v>
-      </c>
-      <c r="E9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" t="s">
-        <v>178</v>
-      </c>
-      <c r="H9" t="s">
-        <v>179</v>
-      </c>
-      <c r="I9" t="s">
-        <v>180</v>
-      </c>
-      <c r="J9" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>182</v>
-      </c>
-      <c r="B10" t="s">
-        <v>183</v>
-      </c>
-      <c r="C10" s="3">
-        <v>38175</v>
-      </c>
-      <c r="D10" t="s">
-        <v>169</v>
-      </c>
-      <c r="E10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" t="s">
-        <v>184</v>
-      </c>
-      <c r="H10" t="s">
-        <v>185</v>
-      </c>
-      <c r="I10" t="s">
-        <v>186</v>
-      </c>
-      <c r="J10" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>188</v>
-      </c>
-      <c r="B11" t="s">
-        <v>189</v>
-      </c>
-      <c r="C11" t="s">
-        <v>190</v>
-      </c>
-      <c r="D11" t="s">
-        <v>169</v>
-      </c>
-      <c r="E11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" t="s">
-        <v>191</v>
-      </c>
-      <c r="H11" t="s">
-        <v>192</v>
-      </c>
-      <c r="I11" t="s">
-        <v>193</v>
-      </c>
-      <c r="J11" t="s">
-        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -1901,10 +1609,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="A12" sqref="A12:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,98 +1838,6 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>168</v>
-      </c>
-      <c r="B12" t="s">
-        <v>195</v>
-      </c>
-      <c r="C12" t="s">
-        <v>196</v>
-      </c>
-      <c r="D12" s="3">
-        <v>43927</v>
-      </c>
-      <c r="E12" t="s">
-        <v>197</v>
-      </c>
-      <c r="F12" t="s">
-        <v>198</v>
-      </c>
-      <c r="G12" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>175</v>
-      </c>
-      <c r="B13" t="s">
-        <v>200</v>
-      </c>
-      <c r="C13" t="s">
-        <v>201</v>
-      </c>
-      <c r="D13" s="3">
-        <v>43288</v>
-      </c>
-      <c r="E13" t="s">
-        <v>202</v>
-      </c>
-      <c r="F13" t="s">
-        <v>203</v>
-      </c>
-      <c r="G13" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B14" t="s">
-        <v>205</v>
-      </c>
-      <c r="C14" t="s">
-        <v>206</v>
-      </c>
-      <c r="D14" s="3">
-        <v>43288</v>
-      </c>
-      <c r="E14" t="s">
-        <v>202</v>
-      </c>
-      <c r="F14" t="s">
-        <v>207</v>
-      </c>
-      <c r="G14" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>189</v>
-      </c>
-      <c r="B15" t="s">
-        <v>209</v>
-      </c>
-      <c r="C15" t="s">
-        <v>210</v>
-      </c>
-      <c r="D15" t="s">
-        <v>211</v>
-      </c>
-      <c r="E15" s="3">
-        <v>43558</v>
-      </c>
-      <c r="F15" t="s">
-        <v>212</v>
-      </c>
-      <c r="G15" t="s">
-        <v>213</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2230,10 +1846,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2243,11 +1859,11 @@
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>106</v>
       </c>
@@ -2258,7 +1874,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
@@ -2277,11 +1893,8 @@
       <c r="F4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
@@ -2298,11 +1911,8 @@
       <c r="F5" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="G5">
-        <v>86553140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
@@ -2319,11 +1929,8 @@
       <c r="F6" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="G6">
-        <v>91874123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>44</v>
       </c>
@@ -2339,43 +1946,6 @@
       <c r="E7" s="14"/>
       <c r="F7" s="14" t="s">
         <v>131</v>
-      </c>
-      <c r="G7">
-        <v>88564432</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>215</v>
-      </c>
-      <c r="C8" s="3">
-        <v>44814</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>217</v>
-      </c>
-      <c r="C9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="G9">
-        <v>83992669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>